<commit_message>
TRIM commands in templates to avoid double spaces
</commit_message>
<xml_diff>
--- a/Load/ontology/script/aggregates_over_multiple_assays_detection_template.xlsx
+++ b/Load/ontology/script/aggregates_over_multiple_assays_detection_template.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{43F13A67-7DE1-6B43-87BD-9B4C50AA6C2A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD8B1BB-B143-9241-9FDD-D65013713333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,10 +1045,10 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="H3" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="S1" sqref="S1"/>
+      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="52" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1163,27 +1163,27 @@
         <v>12</v>
       </c>
       <c r="N3" s="2" t="str">
-        <f>IF($D3&lt;&gt;"","Mean ","Any ")&amp;IF($H3="",$G3,"")
+        <f>TRIM(IF($D3&lt;&gt;"","Mean ","Any ")&amp;IF($H3="",$G3,"")
 &amp;IF($H3&lt;&gt;"",$H3,"")
 &amp;IF(AND($L3="LT",I3="ST")," LT-neg ST-pos",
 IF($I3&lt;&gt;""," "&amp;$I3,"")
 &amp;IF(OR($I3="LT",$I3="ST",$I3&lt;&gt;""),"-pos","")
 &amp;IF($K3&lt;&gt;""," "&amp;$K3,"")
 &amp;IF($J3&lt;&gt;""," "&amp;$J3&amp;"-pos","")
-&amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg",""))&amp;IF($D3="",""," "&amp;$D3)&amp;", by "&amp;$C3</f>
+&amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg",""))&amp;IF($D3="",""," "&amp;$D3)&amp;", by "&amp;$C3)</f>
         <v>Any Vibrio cholerae, by ELISA</v>
       </c>
       <c r="O3" s="2" t="str">
-        <f>IF($I3="",IF($H3="",$G3,$H3),$I3)&amp;" aggregate data"</f>
+        <f>TRIM(IF($I3="",IF($H3="",$G3,$H3),$I3)&amp;" aggregate data")</f>
         <v>Vibrio cholerae aggregate data</v>
       </c>
       <c r="P3" s="2" t="str">
-        <f t="shared" ref="P3" si="0">IF($E3="Eukaryota","Eukaryote",$E3)&amp;" in "&amp;$B3&amp;" aggregate data"</f>
-        <v>Bacteria in stool aggregate data</v>
+        <f>TRIM(IF($E3="Eukaryota","Eukaryote",$E3)&amp;" in "&amp;$B3&amp;" detection aggregate data")</f>
+        <v>Bacteria in stool detection aggregate data</v>
       </c>
       <c r="Q3" s="2" t="str">
-        <f t="shared" ref="Q3:Q4" si="1">"Aggregate organism in "&amp;$B3&amp;" data"</f>
-        <v>Aggregate organism in stool data</v>
+        <f>TRIM("Aggregate organism in "&amp;$B3&amp;" detection data")</f>
+        <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
     <row r="4" spans="1:19" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -1203,27 +1203,27 @@
         <v>17</v>
       </c>
       <c r="N4" s="2" t="str">
-        <f t="shared" ref="N4:N13" si="2">IF($D4&lt;&gt;"","Mean ","Any ")&amp;IF($H4="",$G4,"")
+        <f t="shared" ref="N4:N13" si="0">TRIM(IF($D4&lt;&gt;"","Mean ","Any ")&amp;IF($H4="",$G4,"")
 &amp;IF($H4&lt;&gt;"",$H4,"")
 &amp;IF(AND($L4="LT",I4="ST")," LT-neg ST-pos",
 IF($I4&lt;&gt;""," "&amp;$I4,"")
 &amp;IF(OR($I4="LT",$I4="ST",$I4&lt;&gt;""),"-pos","")
 &amp;IF($K4&lt;&gt;""," "&amp;$K4,"")
 &amp;IF($J4&lt;&gt;""," "&amp;$J4&amp;"-pos","")
-&amp;IF($L4&lt;&gt;""," "&amp;$L4&amp;"-neg",""))&amp;IF($D4="",""," "&amp;$D4)&amp;", by "&amp;$C4</f>
+&amp;IF($L4&lt;&gt;""," "&amp;$L4&amp;"-neg",""))&amp;IF($D4="",""," "&amp;$D4)&amp;", by "&amp;$C4)</f>
         <v>Any Adenovirus, by ELISA</v>
       </c>
       <c r="O4" s="2" t="str">
-        <f t="shared" ref="O4:O9" si="3">IF($I4="",IF($H4="",$G4,$H4),$I4)&amp;" aggregate data"</f>
+        <f t="shared" ref="O4:O13" si="1">TRIM(IF($I4="",IF($H4="",$G4,$H4),$I4)&amp;" aggregate data")</f>
         <v>Adenovirus aggregate data</v>
       </c>
       <c r="P4" s="2" t="str">
-        <f t="shared" ref="P4:P8" si="4">IF($E4="Eukaryota","Eukaryote",$E4)&amp;" in "&amp;$B4&amp;" detection aggregate data"</f>
+        <f t="shared" ref="P4:P13" si="2">TRIM(IF($E4="Eukaryota","Eukaryote",$E4)&amp;" in "&amp;$B4&amp;" detection aggregate data")</f>
         <v>Virus in stool detection aggregate data</v>
       </c>
       <c r="Q4" s="2" t="str">
-        <f t="shared" si="1"/>
-        <v>Aggregate organism in stool data</v>
+        <f t="shared" ref="Q4:Q13" si="3">TRIM("Aggregate organism in "&amp;$B4&amp;" detection data")</f>
+        <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
     <row r="5" spans="1:19" ht="52" customHeight="1" x14ac:dyDescent="0.2">
@@ -1246,19 +1246,19 @@
         <v>53</v>
       </c>
       <c r="N5" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Mean Schistosoma mansoni count eggs per gram, by microscopy</v>
+      </c>
+      <c r="O5" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Schistosoma mansoni aggregate data</v>
+      </c>
+      <c r="P5" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Mean Schistosoma mansoni count eggs per gram, by microscopy</v>
-      </c>
-      <c r="O5" s="2" t="str">
+        <v>Eukaryote in urine detection aggregate data</v>
+      </c>
+      <c r="Q5" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Schistosoma mansoni aggregate data</v>
-      </c>
-      <c r="P5" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Eukaryote in urine detection aggregate data</v>
-      </c>
-      <c r="Q5" s="2" t="str">
-        <f>"Aggregate organism in "&amp;$B5&amp;" detection data"</f>
         <v>Aggregate organism in urine detection data</v>
       </c>
     </row>
@@ -1279,19 +1279,19 @@
         <v>18</v>
       </c>
       <c r="N6" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any Ancylostoma, by TAC</v>
+      </c>
+      <c r="O6" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Ancylostoma aggregate data</v>
+      </c>
+      <c r="P6" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any Ancylostoma, by TAC</v>
-      </c>
-      <c r="O6" s="2" t="str">
+        <v>Eukaryote in stool detection aggregate data</v>
+      </c>
+      <c r="Q6" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Ancylostoma aggregate data</v>
-      </c>
-      <c r="P6" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Eukaryote in stool detection aggregate data</v>
-      </c>
-      <c r="Q6" s="2" t="str">
-        <f t="shared" ref="Q6:Q13" si="5">"Aggregate organism in "&amp;$B6&amp;" detection data"</f>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1312,19 +1312,19 @@
         <v>20</v>
       </c>
       <c r="N7" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any Campylobacter, by ELISA</v>
+      </c>
+      <c r="O7" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Campylobacter aggregate data</v>
+      </c>
+      <c r="P7" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any Campylobacter, by ELISA</v>
-      </c>
-      <c r="O7" s="2" t="str">
+        <v>Bacteria in stool detection aggregate data</v>
+      </c>
+      <c r="Q7" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Campylobacter aggregate data</v>
-      </c>
-      <c r="P7" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Bacteria in stool detection aggregate data</v>
-      </c>
-      <c r="Q7" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1345,19 +1345,19 @@
         <v>41</v>
       </c>
       <c r="N8" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any Norovirus GII, by RT-PCR</v>
+      </c>
+      <c r="O8" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Norovirus GII aggregate data</v>
+      </c>
+      <c r="P8" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any Norovirus GII, by RT-PCR</v>
-      </c>
-      <c r="O8" s="2" t="str">
+        <v>Virus in stool detection aggregate data</v>
+      </c>
+      <c r="Q8" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Norovirus GII aggregate data</v>
-      </c>
-      <c r="P8" s="2" t="str">
-        <f t="shared" si="4"/>
-        <v>Virus in stool detection aggregate data</v>
-      </c>
-      <c r="Q8" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1378,19 +1378,19 @@
         <v>23</v>
       </c>
       <c r="N9" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any Chikungunya, by SD Bioline IgM ELISA</v>
+      </c>
+      <c r="O9" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Chikungunya aggregate data</v>
+      </c>
+      <c r="P9" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any Chikungunya, by SD Bioline IgM ELISA</v>
-      </c>
-      <c r="O9" s="2" t="str">
+        <v>Virus in stool detection aggregate data</v>
+      </c>
+      <c r="Q9" s="2" t="str">
         <f t="shared" si="3"/>
-        <v>Chikungunya aggregate data</v>
-      </c>
-      <c r="P9" s="2" t="str">
-        <f t="shared" ref="P9:P12" si="6">IF($E9="Eukaryota","Eukaryote",$E9)&amp;" in "&amp;$B9&amp;" detection aggregate data"</f>
-        <v>Virus in stool detection aggregate data</v>
-      </c>
-      <c r="Q9" s="2" t="str">
-        <f t="shared" si="5"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1420,19 +1420,19 @@
         <v>32</v>
       </c>
       <c r="N10" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any ETEC LT-pos ST-neg, by PCR</v>
+      </c>
+      <c r="O10" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>LT aggregate data</v>
+      </c>
+      <c r="P10" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any ETEC LT-pos ST-neg, by PCR</v>
-      </c>
-      <c r="O10" s="2" t="str">
-        <f t="shared" ref="O10:O12" si="7">$F10&amp;" in "&amp;$B10&amp;" aggregate data"</f>
-        <v>Escherichia in stool aggregate data</v>
-      </c>
-      <c r="P10" s="2" t="str">
-        <f t="shared" si="6"/>
         <v>Bacteria in stool detection aggregate data</v>
       </c>
       <c r="Q10" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1456,19 +1456,19 @@
         <v>37</v>
       </c>
       <c r="N11" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any STEC, by PCR</v>
+      </c>
+      <c r="O11" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>STEC aggregate data</v>
+      </c>
+      <c r="P11" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any STEC, by PCR</v>
-      </c>
-      <c r="O11" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Escherichia in stool aggregate data</v>
-      </c>
-      <c r="P11" s="2" t="str">
-        <f t="shared" si="6"/>
         <v>Bacteria in stool detection aggregate data</v>
       </c>
       <c r="Q11" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1501,19 +1501,19 @@
         <v>57</v>
       </c>
       <c r="N12" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any STEC stx1-pos or stx2-pos, by PCR</v>
+      </c>
+      <c r="O12" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>stx1 aggregate data</v>
+      </c>
+      <c r="P12" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any STEC stx1-pos or stx2-pos, by PCR</v>
-      </c>
-      <c r="O12" s="2" t="str">
-        <f t="shared" si="7"/>
-        <v>Escherichia in stool aggregate data</v>
-      </c>
-      <c r="P12" s="2" t="str">
-        <f t="shared" si="6"/>
         <v>Bacteria in stool detection aggregate data</v>
       </c>
       <c r="Q12" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>
@@ -1534,19 +1534,19 @@
         <v>46</v>
       </c>
       <c r="N13" s="2" t="str">
+        <f t="shared" si="0"/>
+        <v>Any Hookworm, by microscopy</v>
+      </c>
+      <c r="O13" s="2" t="str">
+        <f t="shared" si="1"/>
+        <v>Hookworm aggregate data</v>
+      </c>
+      <c r="P13" s="2" t="str">
         <f t="shared" si="2"/>
-        <v>Any Hookworm, by microscopy</v>
-      </c>
-      <c r="O13" s="2" t="str">
-        <f>$F13&amp;" in "&amp;$B13&amp;" aggregate data"</f>
-        <v>Ancylostomatoidea in stool aggregate data</v>
-      </c>
-      <c r="P13" s="2" t="str">
-        <f>IF($E13="Eukaryota","Eukaryote",$E13)&amp;" in "&amp;$B13&amp;" detection aggregate data"</f>
         <v>Eukaryote in stool detection aggregate data</v>
       </c>
       <c r="Q13" s="2" t="str">
-        <f t="shared" si="5"/>
+        <f t="shared" si="3"/>
         <v>Aggregate organism in stool detection data</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Templates updated to put -pos before -neg in label
</commit_message>
<xml_diff>
--- a/Load/ontology/script/aggregates_over_multiple_assays_detection_template.xlsx
+++ b/Load/ontology/script/aggregates_over_multiple_assays_detection_template.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/ontology/script/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jjudkins/Documents/GitHub/ApiCommonData/Load/ontology/script/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD8B1BB-B143-9241-9FDD-D65013713333}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3F733FF6-D3B3-6041-BEA4-4F8E8EBFCB30}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="33600" windowHeight="19340" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1045,10 +1045,10 @@
   <dimension ref="A1:S14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="G8" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="C6" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
-      <selection pane="bottomRight" activeCell="R6" sqref="R6"/>
+      <selection pane="bottomRight" activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="52" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1165,12 +1165,11 @@
       <c r="N3" s="2" t="str">
         <f>TRIM(IF($D3&lt;&gt;"","Mean ","Any ")&amp;IF($H3="",$G3,"")
 &amp;IF($H3&lt;&gt;"",$H3,"")
-&amp;IF(AND($L3="LT",I3="ST")," LT-neg ST-pos",
-IF($I3&lt;&gt;""," "&amp;$I3,"")
+&amp;IF($I3&lt;&gt;""," "&amp;$I3,"")
 &amp;IF(OR($I3="LT",$I3="ST",$I3&lt;&gt;""),"-pos","")
 &amp;IF($K3&lt;&gt;""," "&amp;$K3,"")
 &amp;IF($J3&lt;&gt;""," "&amp;$J3&amp;"-pos","")
-&amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg",""))&amp;IF($D3="",""," "&amp;$D3)&amp;", by "&amp;$C3)</f>
+&amp;IF($L3&lt;&gt;""," "&amp;$L3&amp;"-neg","")&amp;IF($D3="",""," "&amp;$D3)&amp;", by "&amp;$C3)</f>
         <v>Any Vibrio cholerae, by ELISA</v>
       </c>
       <c r="O3" s="2" t="str">
@@ -1205,12 +1204,11 @@
       <c r="N4" s="2" t="str">
         <f t="shared" ref="N4:N13" si="0">TRIM(IF($D4&lt;&gt;"","Mean ","Any ")&amp;IF($H4="",$G4,"")
 &amp;IF($H4&lt;&gt;"",$H4,"")
-&amp;IF(AND($L4="LT",I4="ST")," LT-neg ST-pos",
-IF($I4&lt;&gt;""," "&amp;$I4,"")
+&amp;IF($I4&lt;&gt;""," "&amp;$I4,"")
 &amp;IF(OR($I4="LT",$I4="ST",$I4&lt;&gt;""),"-pos","")
 &amp;IF($K4&lt;&gt;""," "&amp;$K4,"")
 &amp;IF($J4&lt;&gt;""," "&amp;$J4&amp;"-pos","")
-&amp;IF($L4&lt;&gt;""," "&amp;$L4&amp;"-neg",""))&amp;IF($D4="",""," "&amp;$D4)&amp;", by "&amp;$C4)</f>
+&amp;IF($L4&lt;&gt;""," "&amp;$L4&amp;"-neg","")&amp;IF($D4="",""," "&amp;$D4)&amp;", by "&amp;$C4)</f>
         <v>Any Adenovirus, by ELISA</v>
       </c>
       <c r="O4" s="2" t="str">
@@ -1414,18 +1412,18 @@
         <v>30</v>
       </c>
       <c r="I10" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="L10" s="1" t="s">
         <v>31</v>
-      </c>
-      <c r="L10" s="1" t="s">
-        <v>32</v>
       </c>
       <c r="N10" s="2" t="str">
         <f t="shared" si="0"/>
-        <v>Any ETEC LT-pos ST-neg, by PCR</v>
+        <v>Any ETEC ST-pos LT-neg, by PCR</v>
       </c>
       <c r="O10" s="2" t="str">
         <f t="shared" si="1"/>
-        <v>LT aggregate data</v>
+        <v>ST aggregate data</v>
       </c>
       <c r="P10" s="2" t="str">
         <f t="shared" si="2"/>

</xml_diff>